<commit_message>
update smk and sky
Signed-off-by: DingWB <ding.wu.bin.gm@gmail.com>
</commit_message>
<xml_diff>
--- a/bmzip/data/structure.xlsx
+++ b/bmzip/data/structure.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wding/Projects/Github/bmzip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wding/Projects/Github/bmzip/bmzip/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7001ECD9-F7E7-9D41-AA14-56B18F918EA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D7D499-4706-CA49-9C1C-E90307ED208C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{44CE7D83-8765-4041-8F58-EDBF1CDF0E40}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{44CE7D83-8765-4041-8F58-EDBF1CDF0E40}"/>
   </bookViews>
   <sheets>
-    <sheet name="structrure" sheetId="1" r:id="rId1"/>
-    <sheet name="bmi" sheetId="2" r:id="rId2"/>
+    <sheet name="Summary" sheetId="6" r:id="rId1"/>
+    <sheet name="design" sheetId="1" r:id="rId2"/>
+    <sheet name="chunk" sheetId="5" r:id="rId3"/>
+    <sheet name="compare" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="113">
   <si>
     <t>EOF</t>
   </si>
@@ -366,12 +369,102 @@
       <t>(&gt; header_size)</t>
     </r>
   </si>
+  <si>
+    <t>allc</t>
+  </si>
+  <si>
+    <t>ballc</t>
+  </si>
+  <si>
+    <t>mz</t>
+  </si>
+  <si>
+    <t>.tsv.gz</t>
+  </si>
+  <si>
+    <t>allcools</t>
+  </si>
+  <si>
+    <t>ballcools</t>
+  </si>
+  <si>
+    <t>bmzip</t>
+  </si>
+  <si>
+    <t>.ballc</t>
+  </si>
+  <si>
+    <t>.mz</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Compression algorithm</t>
+  </si>
+  <si>
+    <t>bgzip</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Support Random Access ?</t>
+  </si>
+  <si>
+    <t>chrom</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>strand</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>mc</t>
+  </si>
+  <si>
+    <t>cov</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Reference file for all cells</t>
+  </si>
+  <si>
+    <t>Fields (stored in each cell)</t>
+  </si>
+  <si>
+    <t>Chunk 1</t>
+  </si>
+  <si>
+    <t>Need extra index file for query?</t>
+  </si>
+  <si>
+    <t>Quickly Merge?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,8 +523,52 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,8 +593,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -879,11 +1022,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -927,9 +1081,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -999,121 +1150,199 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1429,11 +1658,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FCEFFC-7AFE-1449-99C7-256FAD9190A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA3E2C7-2393-9E43-8006-12262B9CD5B7}">
   <dimension ref="B1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1450,333 +1679,333 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="38" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="30"/>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="26">
         <v>5</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="30"/>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="26">
         <v>4</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="31">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="30"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="26">
         <v>8</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="31"/>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <v>2</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="31"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="30"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>1</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="25"/>
-      <c r="C9" s="47" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="48"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="76"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="30"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="26">
         <v>1</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="30"/>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="74"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="25"/>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>1</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="25"/>
-      <c r="C15" s="29" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="49"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
-      <c r="C17" s="29" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="26">
         <v>1</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="25"/>
-      <c r="C18" s="45" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" s="24" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="21">
         <v>1</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="14" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
     </row>
     <row r="22" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="77"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="67"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="4" t="s">
         <v>31</v>
       </c>
@@ -1794,43 +2023,43 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="37"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="34">
         <v>8</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G24" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="37"/>
-      <c r="C26" s="66" t="s">
+      <c r="B26" s="36"/>
+      <c r="C26" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="68"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="58"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="37"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="14" t="s">
         <v>24</v>
       </c>
@@ -1848,7 +2077,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="37"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="13" t="s">
         <v>20</v>
       </c>
@@ -1866,7 +2095,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="37"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="12" t="s">
         <v>17</v>
       </c>
@@ -1884,7 +2113,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="37"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="12" t="s">
         <v>13</v>
       </c>
@@ -1900,63 +2129,63 @@
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="2:7" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="62"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
     </row>
     <row r="32" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="37"/>
-      <c r="C32" s="63" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="65"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="55"/>
     </row>
     <row r="33" spans="2:7" ht="13" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="37"/>
-      <c r="C33" s="69" t="s">
+      <c r="B33" s="36"/>
+      <c r="C33" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
     </row>
     <row r="34" spans="2:7" ht="14" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="37"/>
-      <c r="C34" s="66" t="s">
+      <c r="B34" s="36"/>
+      <c r="C34" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="68"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58"/>
     </row>
     <row r="35" spans="2:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="60"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="62"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
     </row>
     <row r="36" spans="2:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="39"/>
-      <c r="C36" s="40" t="s">
+      <c r="B36" s="40"/>
+      <c r="C36" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="38"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="7" t="s">
         <v>9</v>
       </c>
@@ -1974,7 +2203,7 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="37"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="4" t="s">
         <v>7</v>
       </c>
@@ -1992,17 +2221,17 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="71" t="s">
+      <c r="B39" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="73"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="63"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="37"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="4" t="s">
         <v>5</v>
       </c>
@@ -2020,119 +2249,529 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="37"/>
-      <c r="C41" s="72" t="s">
+      <c r="B41" s="36"/>
+      <c r="C41" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="73"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="63"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="37"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="35">
+      <c r="F42" s="34">
         <v>1</v>
       </c>
-      <c r="G42" s="36">
+      <c r="G42" s="35">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="37"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="35" t="s">
+      <c r="F43" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="36" t="s">
+      <c r="G43" s="35" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="74"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
     </row>
     <row r="45" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="55"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
     </row>
     <row r="46" spans="2:7" ht="11" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="52" t="s">
+      <c r="B46" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
     </row>
     <row r="47" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="55"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="45"/>
     </row>
     <row r="48" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
     </row>
     <row r="49" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
     <mergeCell ref="B46:G46"/>
     <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C25:G25"/>
     <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B31:G31"/>
     <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
     <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C41:G41"/>
     <mergeCell ref="B35:G35"/>
     <mergeCell ref="C36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="B16:G16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FCEFFC-7AFE-1449-99C7-256FAD9190A7}">
+  <dimension ref="B1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="29"/>
+      <c r="C3" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="26">
+        <v>5</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="29"/>
+      <c r="C4" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="26">
+        <v>4</v>
+      </c>
+      <c r="G4" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="29"/>
+      <c r="C5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="26">
+        <v>8</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="30"/>
+      <c r="C6" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="26">
+        <v>2</v>
+      </c>
+      <c r="G6" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="30"/>
+      <c r="C7" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="29"/>
+      <c r="C8" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="26">
+        <v>1</v>
+      </c>
+      <c r="G8" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="24"/>
+      <c r="C9" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="76"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="29"/>
+      <c r="C10" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="26">
+        <v>1</v>
+      </c>
+      <c r="G10" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="29"/>
+      <c r="C11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="24"/>
+      <c r="C13" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="74"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="24"/>
+      <c r="C14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="G14" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="24"/>
+      <c r="C15" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="77"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="29"/>
+      <c r="C17" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="26">
+        <v>1</v>
+      </c>
+      <c r="G17" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="24"/>
+      <c r="C18" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="24"/>
+      <c r="C19" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="21">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="14" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+    </row>
+    <row r="22" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+    </row>
+    <row r="23" spans="2:7" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+    </row>
+    <row r="24" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+    </row>
+    <row r="25" spans="2:7" ht="11" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+    </row>
+    <row r="26" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+    </row>
+    <row r="27" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+    </row>
+    <row r="28" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="14">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="C13:G13"/>
@@ -2140,19 +2779,664 @@
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD7F809-2C45-334C-86C1-7E13CE08E5BE}">
+  <dimension ref="B1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="41"/>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="36"/>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="34">
+        <v>8</v>
+      </c>
+      <c r="G4" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="36"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
+    </row>
+    <row r="6" spans="2:7" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="36"/>
+      <c r="C6" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="36"/>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="14">
+        <v>2</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="36"/>
+      <c r="C8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="36"/>
+      <c r="C9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="36"/>
+      <c r="C10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="2:7" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
+    </row>
+    <row r="12" spans="2:7" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
+      <c r="C12" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
+    </row>
+    <row r="13" spans="2:7" ht="13" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="36"/>
+      <c r="C13" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
+    </row>
+    <row r="14" spans="2:7" ht="14" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="36"/>
+      <c r="C14" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
+    </row>
+    <row r="15" spans="2:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
+    </row>
+    <row r="16" spans="2:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="40"/>
+      <c r="C16" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="37"/>
+      <c r="C17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="7">
+        <v>8</v>
+      </c>
+      <c r="G17" s="6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="36"/>
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="4">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="63"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="36"/>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="4">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="36"/>
+      <c r="C21" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="63"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="36"/>
+      <c r="C22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="34">
+        <v>1</v>
+      </c>
+      <c r="G22" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="36"/>
+      <c r="C23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8BC542-D28C-3441-A474-4F512B93E05C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.5" style="81" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="80" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="80" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="80" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="80"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="89"/>
+      <c r="B1" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="82" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347E119F-81BE-9B46-B433-10B817C4C418}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="97"/>
+      <c r="B1" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="J1" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+    </row>
+    <row r="2" spans="1:13" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="83"/>
+      <c r="B2" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="101" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="101" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="21" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="92" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="102" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+    </row>
+    <row r="4" spans="1:13" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" s="93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="L5" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="100" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J3:M3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>